<commit_message>
all graph is updated
</commit_message>
<xml_diff>
--- a/database/MainDataset.xlsx
+++ b/database/MainDataset.xlsx
@@ -407,17 +407,17 @@
   <dimension ref="A1:F1458"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>